<commit_message>
fix: added primary/final energy carrier mapping for electricity
</commit_message>
<xml_diff>
--- a/import/raw_data/mapping__final_energy_carrier__primary_energy_carrier.xlsx
+++ b/import/raw_data/mapping__final_energy_carrier__primary_energy_carrier.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Python_env\workspace\micat\back_end\import\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenz/Projekte/micat/import/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0647132-A9EC-1A4A-9FB1-50BEF8D909FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="19170" windowHeight="6870"/>
+    <workbookView xWindow="960" yWindow="760" windowWidth="19580" windowHeight="13400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -49,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,7 +82,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -369,20 +359,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -393,7 +383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -401,10 +391,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-999</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -415,7 +405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -426,7 +416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -437,7 +427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -448,7 +438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -459,7 +449,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -476,6 +466,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">mapping</Type>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010081027A5C4AB68A40A5017F28CDCC410C" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6a99bad85733394ec9884d367e30f22e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca47701c-f272-4f81-9665-1c7dbebc0776" xmlns:ns3="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7c78837beb47b266e55ad3edbd611a71" ns2:_="" ns3:_="">
     <xsd:import namespace="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
@@ -722,18 +724,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">mapping</Type>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -744,6 +734,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9043B7D-778A-476D-BCA3-6C45575D69C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
+    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{756BA430-C83A-473F-B636-66FBC9F59B79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -762,17 +763,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9043B7D-778A-476D-BCA3-6C45575D69C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
-    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2F95140-1929-46DA-9812-5261B0E3CEFD}">
   <ds:schemaRefs>

</xml_diff>